<commit_message>
jacky seed complete fucking hell
</commit_message>
<xml_diff>
--- a/styleMatch.xlsx
+++ b/styleMatch.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{627B9EE9-764E-483B-AEE0-2151F35BB934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16E191D7-7981-42C6-A5DD-F55CACCA211F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,27 +32,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
-  <si>
-    <t>oval</t>
-  </si>
-  <si>
-    <t>heart</t>
-  </si>
-  <si>
-    <t>round</t>
-  </si>
-  <si>
-    <t>square</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="47">
+  <si>
+    <t>Oval</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Square</t>
   </si>
   <si>
     <t>oblong</t>
   </si>
   <si>
-    <t>Bob cut hairstyle</t>
-  </si>
-  <si>
-    <t>Afro hairstyle</t>
+    <t>Bob Cut Hairstyle</t>
+  </si>
+  <si>
+    <t>Afro Hairstyle</t>
   </si>
   <si>
     <t>Bowl Cut Hairstyle</t>
@@ -84,13 +85,10 @@
     <t>Dreadlocks Hairstyle</t>
   </si>
   <si>
-    <t xml:space="preserve">Curtained Hair Hairstyle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crew Cut Hairstyle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dido Flip Hairstyle </t>
+    <t>Curtained Hair Hairstyle</t>
+  </si>
+  <si>
+    <t>Dido Flip Hairstyle</t>
   </si>
   <si>
     <t>Frosted Tips Hairstyle</t>
@@ -108,7 +106,7 @@
     <t>Jewfro Hairstyle</t>
   </si>
   <si>
-    <t xml:space="preserve">Psychobilly Wedge Hairstyle </t>
+    <t>Psychobilly Wedge Hairstyle</t>
   </si>
   <si>
     <t>French Braid Hairstyle</t>
@@ -144,7 +142,7 @@
     <t>Shingle Bob Hairstyle</t>
   </si>
   <si>
-    <t xml:space="preserve">Harvard Clip Hairstyle </t>
+    <t>Harvard Clip Hairstyle</t>
   </si>
   <si>
     <t>Marcel Waves Hairstyle</t>
@@ -168,10 +166,10 @@
     <t>Taper Cut Hairstyle</t>
   </si>
   <si>
+    <t>Short Hair Hairstyle</t>
+  </si>
+  <si>
     <t>The Rachel Hairstyle</t>
-  </si>
-  <si>
-    <t>Short Hair Hairstyle</t>
   </si>
   <si>
     <t>Updo Hairstyle</t>
@@ -532,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F85705-C449-4E28-AF4B-F5F58B22A8B8}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,6 +614,96 @@
         <v>11</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
@@ -652,19 +740,19 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -675,10 +763,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -689,33 +777,33 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -723,16 +811,16 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -740,16 +828,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -757,195 +845,198 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
         <v>43</v>
       </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -955,17 +1046,22 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jacky gen image and posted on front-end
</commit_message>
<xml_diff>
--- a/styleMatch.xlsx
+++ b/styleMatch.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16E191D7-7981-42C6-A5DD-F55CACCA211F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F53335B7-B274-4852-BBDC-E01526205CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="55">
   <si>
     <t>Oval</t>
   </si>
@@ -70,109 +70,133 @@
     <t>Crew Cut Hairstyle</t>
   </si>
   <si>
-    <t>Caesar Cut Hairstyle</t>
-  </si>
-  <si>
-    <t>Crown Braid Hairstyle</t>
-  </si>
-  <si>
-    <t>Cornrows Hairstyle</t>
-  </si>
-  <si>
-    <t>Fade Hairstyle</t>
-  </si>
-  <si>
-    <t>Dreadlocks Hairstyle</t>
-  </si>
-  <si>
-    <t>Curtained Hair Hairstyle</t>
-  </si>
-  <si>
-    <t>Dido Flip Hairstyle</t>
-  </si>
-  <si>
-    <t>Frosted Tips Hairstyle</t>
-  </si>
-  <si>
-    <t>Mohawk Hairstyle</t>
-  </si>
-  <si>
-    <t>Perm Hairstyle</t>
-  </si>
-  <si>
-    <t>Fauxhawk Hairstyle</t>
-  </si>
-  <si>
-    <t>Jewfro Hairstyle</t>
-  </si>
-  <si>
-    <t>Psychobilly Wedge Hairstyle</t>
-  </si>
-  <si>
-    <t>French Braid Hairstyle</t>
-  </si>
-  <si>
-    <t>Liberty Spikes Hairstyle</t>
-  </si>
-  <si>
-    <t>Quiff Hairstyle</t>
-  </si>
-  <si>
-    <t>Full Crown Hairstyle</t>
-  </si>
-  <si>
-    <t>Regular Taper Cut Hairstyle</t>
-  </si>
-  <si>
-    <t>Slicked-Back Hairstyle</t>
-  </si>
-  <si>
-    <t>Hime Cut Hairstyle</t>
-  </si>
-  <si>
-    <t>Ringlets Hairstyle</t>
-  </si>
-  <si>
-    <t>Undercut Hairstyle</t>
-  </si>
-  <si>
-    <t>Jheri Curl Hairstyle</t>
-  </si>
-  <si>
-    <t>Shingle Bob Hairstyle</t>
-  </si>
-  <si>
-    <t>Harvard Clip Hairstyle</t>
-  </si>
-  <si>
-    <t>Marcel Waves Hairstyle</t>
-  </si>
-  <si>
-    <t>High and Tight Hairstyle</t>
-  </si>
-  <si>
-    <t>Finger Waves Hairstyle</t>
-  </si>
-  <si>
-    <t>Spiky Hair Hairstyle</t>
-  </si>
-  <si>
-    <t>Pixie Cut Hairstyle</t>
-  </si>
-  <si>
-    <t>Surfer Hair Hairstyle</t>
-  </si>
-  <si>
-    <t>Taper Cut Hairstyle</t>
-  </si>
-  <si>
-    <t>Short Hair Hairstyle</t>
-  </si>
-  <si>
-    <t>The Rachel Hairstyle</t>
-  </si>
-  <si>
-    <t>Updo Hairstyle</t>
+    <t>bob cut hairstyle</t>
+  </si>
+  <si>
+    <t>afro hairstyle</t>
+  </si>
+  <si>
+    <t>bowl cut hairstyle</t>
+  </si>
+  <si>
+    <t>braid hairstyle</t>
+  </si>
+  <si>
+    <t>chignon hairstyle</t>
+  </si>
+  <si>
+    <t>extensions hairstyle</t>
+  </si>
+  <si>
+    <t>crew cut hairstyle</t>
+  </si>
+  <si>
+    <t>caesar cut hairstyle</t>
+  </si>
+  <si>
+    <t>crown braid hairstyle</t>
+  </si>
+  <si>
+    <t>cornrows hairstyle</t>
+  </si>
+  <si>
+    <t>fade hairstyle</t>
+  </si>
+  <si>
+    <t>dreadlocks hairstyle</t>
+  </si>
+  <si>
+    <t>curtained hair hairstyle</t>
+  </si>
+  <si>
+    <t>dido flip hairstyle</t>
+  </si>
+  <si>
+    <t>frosted tips hairstyle</t>
+  </si>
+  <si>
+    <t>mohawk hairstyle</t>
+  </si>
+  <si>
+    <t>perm hairstyle</t>
+  </si>
+  <si>
+    <t>fauxhawk hairstyle</t>
+  </si>
+  <si>
+    <t>jewfro hairstyle</t>
+  </si>
+  <si>
+    <t>psychobilly wedge hairstyle</t>
+  </si>
+  <si>
+    <t>french braid hairstyle</t>
+  </si>
+  <si>
+    <t>liberty spikes hairstyle</t>
+  </si>
+  <si>
+    <t>quiff hairstyle</t>
+  </si>
+  <si>
+    <t>full crown hairstyle</t>
+  </si>
+  <si>
+    <t>regular taper cut hairstyle</t>
+  </si>
+  <si>
+    <t>slicked-back hairstyle</t>
+  </si>
+  <si>
+    <t>hime cut hairstyle</t>
+  </si>
+  <si>
+    <t>ringlets hairstyle</t>
+  </si>
+  <si>
+    <t>undercut hairstyle</t>
+  </si>
+  <si>
+    <t>jheri curl hairstyle</t>
+  </si>
+  <si>
+    <t>shingle bob hairstyle</t>
+  </si>
+  <si>
+    <t>harvard clip hairstyle</t>
+  </si>
+  <si>
+    <t>marcel waves hairstyle</t>
+  </si>
+  <si>
+    <t>high and tight hairstyle</t>
+  </si>
+  <si>
+    <t>finger waves hairstyle</t>
+  </si>
+  <si>
+    <t>spiky hair hairstyle</t>
+  </si>
+  <si>
+    <t>pixie cut hairstyle</t>
+  </si>
+  <si>
+    <t>surfer hair hairstyle</t>
+  </si>
+  <si>
+    <t>taper cut hairstyle</t>
+  </si>
+  <si>
+    <t>short hair hairstyle</t>
+  </si>
+  <si>
+    <t>the rachel hairstyle</t>
+  </si>
+  <si>
+    <t>updo hairstyle</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -623,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,6 +658,10 @@
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -655,413 +683,614 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>